<commit_message>
added data dictionary content
</commit_message>
<xml_diff>
--- a/data_dictionary/data_dictionary.xlsx
+++ b/data_dictionary/data_dictionary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\janni\Dropbox\university\13 Semester bis zum Lebensende\2021_01 FundMapper\repo\data_dictionary\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BE08C6A-1DBC-4DC3-B3C1-3DAF2CD1EDB9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCA71507-A726-49B6-A44C-6DC6BE3F3426}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="class_data" sheetId="1" r:id="rId1"/>
@@ -51,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="204">
   <si>
     <t>series_id</t>
   </si>
@@ -421,12 +421,255 @@
   <si>
     <t>Description</t>
   </si>
+  <si>
+    <t>The filing type, i.e. N-MFP, N-MFP2</t>
+  </si>
+  <si>
+    <t>Flag whether the portfolio item is a repurchase agreement</t>
+  </si>
+  <si>
+    <t>list of guarantors</t>
+  </si>
+  <si>
+    <t>identifier for the investment</t>
+  </si>
+  <si>
+    <t>nrsro number</t>
+  </si>
+  <si>
+    <t>flag to indicate whether fund is treating the acquasition as security purchase</t>
+  </si>
+  <si>
+    <t>maturity date of portfolio item</t>
+  </si>
+  <si>
+    <t>rating of portfolio item</t>
+  </si>
+  <si>
+    <t>category of the investment</t>
+  </si>
+  <si>
+    <t>flag on whether the asset is considered easily liquididated within a week</t>
+  </si>
+  <si>
+    <t>flag on whether the asset is considered easily liquididated within a day</t>
+  </si>
+  <si>
+    <t>CUSIP if availalbe</t>
+  </si>
+  <si>
+    <t>weighted average maturity</t>
+  </si>
+  <si>
+    <t>ISIN</t>
+  </si>
+  <si>
+    <t>LEI of the Issuer</t>
+  </si>
+  <si>
+    <t>flag whether security has enhanced features</t>
+  </si>
+  <si>
+    <t>investment type domain</t>
+  </si>
+  <si>
+    <t>security guarantee flag</t>
+  </si>
+  <si>
+    <t>investment type flag</t>
+  </si>
+  <si>
+    <t>security eligibility flag</t>
+  </si>
+  <si>
+    <t>other unqiue id</t>
+  </si>
+  <si>
+    <t>demands features</t>
+  </si>
+  <si>
+    <t>name of the issuer</t>
+  </si>
+  <si>
+    <t>Name of the issuer + yield</t>
+  </si>
+  <si>
+    <t>flag whether the security is illiquid</t>
+  </si>
+  <si>
+    <t>series id of the fund</t>
+  </si>
+  <si>
+    <t>yield of the security</t>
+  </si>
+  <si>
+    <t>weighted average life of the investment</t>
+  </si>
+  <si>
+    <t>value including value of any sponsor support</t>
+  </si>
+  <si>
+    <t>value exckuding value of any sponsor support</t>
+  </si>
+  <si>
+    <t>% of the entire portfolio</t>
+  </si>
+  <si>
+    <t>date YYYYMM</t>
+  </si>
+  <si>
+    <t>number of issue in portfolio</t>
+  </si>
+  <si>
+    <t>type of investment</t>
+  </si>
+  <si>
+    <t>partition, alias for year YYYY</t>
+  </si>
+  <si>
+    <t>CIK of the fund</t>
+  </si>
+  <si>
+    <t>available for sale securities amortized cost</t>
+  </si>
+  <si>
+    <t>investemnt owned balance principal amount</t>
+  </si>
+  <si>
+    <t>category investment of he collateral</t>
+  </si>
+  <si>
+    <t>filing type of the filing</t>
+  </si>
+  <si>
+    <t>LEI ID of the issuer of the collateral</t>
+  </si>
+  <si>
+    <t>Amount of collateral in $</t>
+  </si>
+  <si>
+    <t>maturity date of collateral</t>
+  </si>
+  <si>
+    <t>name of the collateral issuer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">issuer number </t>
+  </si>
+  <si>
+    <t>coupon or yield</t>
+  </si>
+  <si>
+    <t>value of collateral to the nearest cent</t>
+  </si>
+  <si>
+    <t>collateral value</t>
+  </si>
+  <si>
+    <t>parition, alias for year YYYY</t>
+  </si>
+  <si>
+    <t>Assets sold under agreements to repurchase carrying amounts</t>
+  </si>
+  <si>
+    <t>cash collateral for borrowed securities</t>
+  </si>
+  <si>
+    <t>sub adviser</t>
+  </si>
+  <si>
+    <t>filing type</t>
+  </si>
+  <si>
+    <t>flag for retail funds</t>
+  </si>
+  <si>
+    <t>file information number</t>
+  </si>
+  <si>
+    <t>transfer agent</t>
+  </si>
+  <si>
+    <t>advisor</t>
+  </si>
+  <si>
+    <t>advisor list</t>
+  </si>
+  <si>
+    <t>series id of the class fund share</t>
+  </si>
+  <si>
+    <t>class id</t>
+  </si>
+  <si>
+    <t>person pay fund flag</t>
+  </si>
+  <si>
+    <t>name of the fund paying the expense</t>
+  </si>
+  <si>
+    <t>gross scubscriptions</t>
+  </si>
+  <si>
+    <t>netshare flow</t>
+  </si>
+  <si>
+    <t>minimal investment</t>
+  </si>
+  <si>
+    <t>gross redemptions</t>
+  </si>
+  <si>
+    <t>net asset value per share including capital support aggrement</t>
+  </si>
+  <si>
+    <t>net assets of share class</t>
+  </si>
+  <si>
+    <t>net assets per share</t>
+  </si>
+  <si>
+    <t>net assets per share excluding capital support aggrement</t>
+  </si>
+  <si>
+    <t>seve day net yield</t>
+  </si>
+  <si>
+    <t>partion, alias for year YYYY</t>
+  </si>
+  <si>
+    <t>gross redemptions week 1</t>
+  </si>
+  <si>
+    <t>gross redemptions week 2</t>
+  </si>
+  <si>
+    <t>gross redemptions week 3</t>
+  </si>
+  <si>
+    <t>gross redemptions week 4</t>
+  </si>
+  <si>
+    <t>gross subscriptions week 1</t>
+  </si>
+  <si>
+    <t>number of shares outstanding</t>
+  </si>
+  <si>
+    <t>gross subscriptions week 4</t>
+  </si>
+  <si>
+    <t>gross subscriptions week 3</t>
+  </si>
+  <si>
+    <t>gross subscriptions week 2</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -438,6 +681,12 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -839,8 +1088,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:B1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -885,128 +1134,204 @@
       <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
+      <c r="B2" t="s">
+        <v>181</v>
+      </c>
     </row>
     <row r="3" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>1</v>
       </c>
+      <c r="B3" t="s">
+        <v>182</v>
+      </c>
     </row>
     <row r="4" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>2</v>
       </c>
+      <c r="B4" t="s">
+        <v>183</v>
+      </c>
     </row>
     <row r="5" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
         <v>3</v>
       </c>
+      <c r="B5" t="s">
+        <v>175</v>
+      </c>
     </row>
     <row r="6" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
         <v>4</v>
       </c>
+      <c r="B6" t="s">
+        <v>184</v>
+      </c>
     </row>
     <row r="7" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
         <v>5</v>
       </c>
+      <c r="B7" t="s">
+        <v>154</v>
+      </c>
     </row>
     <row r="8" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
         <v>6</v>
       </c>
+      <c r="B8" t="s">
+        <v>185</v>
+      </c>
     </row>
     <row r="9" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
         <v>7</v>
       </c>
+      <c r="B9" t="s">
+        <v>186</v>
+      </c>
     </row>
     <row r="10" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
         <v>8</v>
       </c>
+      <c r="B10" t="s">
+        <v>187</v>
+      </c>
     </row>
     <row r="11" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
         <v>9</v>
       </c>
+      <c r="B11" t="s">
+        <v>188</v>
+      </c>
     </row>
     <row r="12" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
         <v>10</v>
       </c>
+      <c r="B12" t="s">
+        <v>189</v>
+      </c>
     </row>
     <row r="13" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="s">
         <v>11</v>
       </c>
+      <c r="B13" t="s">
+        <v>190</v>
+      </c>
     </row>
     <row r="14" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
         <v>12</v>
       </c>
+      <c r="B14" t="s">
+        <v>191</v>
+      </c>
     </row>
     <row r="15" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A15" s="4" t="s">
         <v>13</v>
       </c>
+      <c r="B15" t="s">
+        <v>192</v>
+      </c>
     </row>
     <row r="16" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A16" s="4" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B16" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" s="4" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B17" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" s="4" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B18" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" s="4" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B19" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" s="4" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B20" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" s="4" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B21" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" s="4" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B22" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" s="4" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B23" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" s="4" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B24" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" s="4" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B25" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" s="4" t="s">
         <v>24</v>
       </c>
+      <c r="B26" t="s">
+        <v>203</v>
+      </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
 </worksheet>
@@ -1016,7 +1341,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:BF16384"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -1092,35 +1419,56 @@
       <c r="A2" s="4" t="s">
         <v>25</v>
       </c>
+      <c r="B2" t="s">
+        <v>174</v>
+      </c>
     </row>
     <row r="3" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>3</v>
       </c>
+      <c r="B3" t="s">
+        <v>175</v>
+      </c>
     </row>
     <row r="4" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>26</v>
       </c>
+      <c r="B4" t="s">
+        <v>176</v>
+      </c>
     </row>
     <row r="5" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
         <v>27</v>
       </c>
+      <c r="B5" t="s">
+        <v>177</v>
+      </c>
     </row>
     <row r="6" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
         <v>28</v>
       </c>
+      <c r="B6" t="s">
+        <v>178</v>
+      </c>
     </row>
     <row r="7" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
         <v>29</v>
       </c>
+      <c r="B7" t="s">
+        <v>179</v>
+      </c>
     </row>
     <row r="8" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
         <v>30</v>
+      </c>
+      <c r="B8" t="s">
+        <v>180</v>
       </c>
     </row>
     <row r="9" spans="1:58" x14ac:dyDescent="0.3">
@@ -50361,7 +50709,7 @@
   <dimension ref="A1:B17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:B1"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -50382,75 +50730,120 @@
       <c r="A2" s="4" t="s">
         <v>77</v>
       </c>
+      <c r="B2" t="s">
+        <v>161</v>
+      </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>3</v>
       </c>
+      <c r="B3" t="s">
+        <v>162</v>
+      </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>78</v>
       </c>
+      <c r="B4" t="s">
+        <v>163</v>
+      </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
         <v>79</v>
       </c>
+      <c r="B5" t="s">
+        <v>164</v>
+      </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
         <v>80</v>
       </c>
+      <c r="B6" t="s">
+        <v>165</v>
+      </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
         <v>0</v>
       </c>
+      <c r="B7" t="s">
+        <v>148</v>
+      </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
         <v>81</v>
       </c>
+      <c r="B8" t="s">
+        <v>166</v>
+      </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
         <v>82</v>
       </c>
+      <c r="B9" t="s">
+        <v>167</v>
+      </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
         <v>5</v>
       </c>
+      <c r="B10" t="s">
+        <v>154</v>
+      </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
         <v>83</v>
       </c>
+      <c r="B11" t="s">
+        <v>168</v>
+      </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
         <v>84</v>
       </c>
+      <c r="B12" t="s">
+        <v>169</v>
+      </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="s">
         <v>85</v>
       </c>
+      <c r="B13" t="s">
+        <v>170</v>
+      </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
         <v>15</v>
       </c>
+      <c r="B14" t="s">
+        <v>171</v>
+      </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" s="4" t="s">
         <v>86</v>
       </c>
+      <c r="B15" t="s">
+        <v>172</v>
+      </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" s="4" t="s">
         <v>87</v>
+      </c>
+      <c r="B16" t="s">
+        <v>173</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.3">
@@ -50465,8 +50858,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:B44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="B43" sqref="B43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -50487,11 +50880,17 @@
       <c r="A2" s="4" t="s">
         <v>3</v>
       </c>
+      <c r="B2" t="s">
+        <v>123</v>
+      </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>88</v>
       </c>
+      <c r="B3" t="s">
+        <v>124</v>
+      </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
@@ -50502,41 +50901,65 @@
       <c r="A5" s="4" t="s">
         <v>90</v>
       </c>
+      <c r="B5" t="s">
+        <v>125</v>
+      </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
         <v>91</v>
       </c>
+      <c r="B6" t="s">
+        <v>126</v>
+      </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
         <v>92</v>
       </c>
+      <c r="B7" t="s">
+        <v>127</v>
+      </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
         <v>93</v>
       </c>
+      <c r="B8" t="s">
+        <v>128</v>
+      </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
         <v>94</v>
       </c>
+      <c r="B9" t="s">
+        <v>129</v>
+      </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
         <v>95</v>
       </c>
+      <c r="B10" t="s">
+        <v>132</v>
+      </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
         <v>96</v>
       </c>
+      <c r="B11" t="s">
+        <v>130</v>
+      </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
         <v>97</v>
       </c>
+      <c r="B12" t="s">
+        <v>131</v>
+      </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="s">
@@ -50547,6 +50970,9 @@
       <c r="A14" s="4" t="s">
         <v>99</v>
       </c>
+      <c r="B14" t="s">
+        <v>133</v>
+      </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" s="4" t="s">
@@ -50557,141 +50983,222 @@
       <c r="A16" s="4" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B16" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" s="4" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B17" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" s="4" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B18" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" s="4" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B19" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" s="4" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B20" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" s="4" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B21" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" s="4" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B22" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" s="4" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B23" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" s="4" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B24" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" s="4" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B25" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" s="4" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B26" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" s="4" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B27" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" s="4" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B28" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" s="4" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B29" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30" s="4" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B30" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31" s="4" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B31" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32" s="4" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B32" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33" s="4" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B33" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34" s="4" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B34" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35" s="4" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B35" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36" s="4" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B36" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A37" s="4" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B37" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A38" s="4" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B38" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A39" s="4" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B39" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A40" s="4" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B40" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A41" s="4" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B41" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A42" s="4" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B42" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A43" s="3"/>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A44" s="3"/>
     </row>
   </sheetData>

</xml_diff>